<commit_message>
Cashed checks from Logoworks and MSU
</commit_message>
<xml_diff>
--- a/MIACADA Ledger.xlsx
+++ b/MIACADA Ledger.xlsx
@@ -31,13 +31,13 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId14"/>
+    <pivotCache cacheId="1" r:id="rId14"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="358">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -1607,11 +1607,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="702891696"/>
-        <c:axId val="702892256"/>
+        <c:axId val="784364128"/>
+        <c:axId val="784365248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="702891696"/>
+        <c:axId val="784364128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1654,7 +1654,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="702892256"/>
+        <c:crossAx val="784365248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1662,7 +1662,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="702892256"/>
+        <c:axId val="784365248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1713,7 +1713,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="702891696"/>
+        <c:crossAx val="784364128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2571,7 +2571,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5" rowHeaderCaption="Category">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5" rowHeaderCaption="Category">
   <location ref="A80:B89" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" numFmtId="164" showAll="0" defaultSubtotal="0"/>
@@ -4158,8 +4158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5383,6 +5383,9 @@
       </c>
       <c r="C66" s="20" t="s">
         <v>327</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E66" s="3">
         <v>125</v>
@@ -6829,7 +6832,7 @@
   <dimension ref="A1:M786"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6893,13 +6896,13 @@
       <c r="G2" s="3">
         <v>8256.4599999999991</v>
       </c>
-      <c r="H2" s="24">
-        <v>8506.4599999999991</v>
+      <c r="H2" s="3">
+        <v>8381.4599999999991</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3">
         <f>SUM(J2:J35)</f>
-        <v>490.13</v>
+        <v>125</v>
       </c>
       <c r="M2" s="3"/>
     </row>
@@ -6926,11 +6929,9 @@
       </c>
       <c r="H3" s="3">
         <f>IF(D3="C",H2-E3+F3,H2+F3)</f>
-        <v>8381.4599999999991</v>
-      </c>
-      <c r="J3" s="3">
-        <v>125</v>
-      </c>
+        <v>8256.4599999999991</v>
+      </c>
+      <c r="J3" s="3"/>
       <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -6951,7 +6952,7 @@
       </c>
       <c r="H4" s="3">
         <f t="shared" ref="H4:H9" si="0">IF(D4="C",H3-E4+F4,H3+F4)</f>
-        <v>8395.7199999999993</v>
+        <v>8270.7199999999993</v>
       </c>
       <c r="J4" s="3">
         <v>125</v>
@@ -6976,7 +6977,7 @@
       </c>
       <c r="H5" s="3">
         <f t="shared" si="0"/>
-        <v>8424.24</v>
+        <v>8299.24</v>
       </c>
       <c r="J5" s="3"/>
       <c r="M5" s="3"/>
@@ -6999,7 +7000,7 @@
       </c>
       <c r="H6" s="3">
         <f t="shared" si="0"/>
-        <v>8467.02</v>
+        <v>8342.02</v>
       </c>
       <c r="J6" s="24"/>
       <c r="M6" s="3"/>
@@ -7022,11 +7023,9 @@
       </c>
       <c r="H7" s="3">
         <f t="shared" si="0"/>
-        <v>8509.8000000000011</v>
-      </c>
-      <c r="J7" s="3">
-        <v>240.13</v>
-      </c>
+        <v>8384.8000000000011</v>
+      </c>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="22">
@@ -7046,7 +7045,7 @@
       </c>
       <c r="H8" s="3">
         <f t="shared" si="0"/>
-        <v>8538.3200000000015</v>
+        <v>8413.3200000000015</v>
       </c>
       <c r="M8" s="3"/>
     </row>
@@ -7068,7 +7067,7 @@
       </c>
       <c r="H9" s="3">
         <f t="shared" si="0"/>
-        <v>8552.5800000000017</v>
+        <v>8427.5800000000017</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -7094,7 +7093,7 @@
       </c>
       <c r="H10" s="3">
         <f>IF(D10="C",H9-E10+F10,H9+F10)</f>
-        <v>8158.5200000000013</v>
+        <v>8033.5200000000013</v>
       </c>
       <c r="M10" s="3"/>
     </row>
@@ -7114,7 +7113,7 @@
       </c>
       <c r="H11" s="3">
         <f>IF(D11="C",H10-E11+F11,H10+F11)</f>
-        <v>8172.7800000000016</v>
+        <v>8047.7800000000016</v>
       </c>
       <c r="J11" s="3"/>
       <c r="M11" s="3"/>
@@ -7135,7 +7134,7 @@
       </c>
       <c r="H12" s="3">
         <f>IF(G12="","",IF(D12="C",H11-E12+F12,H11+F12))</f>
-        <v>8201.3000000000011</v>
+        <v>8076.300000000002</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -7160,7 +7159,7 @@
       </c>
       <c r="H13" s="3">
         <f t="shared" ref="H13:H76" si="3">IF(G13="","",IF(D13="C",H12-E13+F13,H12+F13))</f>
-        <v>8107.9400000000014</v>
+        <v>7982.9400000000023</v>
       </c>
       <c r="J13" s="23"/>
       <c r="K13" s="23"/>
@@ -7174,6 +7173,9 @@
       </c>
       <c r="C14" s="20" t="s">
         <v>272</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E14" s="3">
         <v>240.13</v>
@@ -7185,7 +7187,7 @@
       </c>
       <c r="H14" s="3">
         <f t="shared" si="3"/>
-        <v>8107.9400000000014</v>
+        <v>7742.8100000000022</v>
       </c>
       <c r="L14" s="3"/>
     </row>
@@ -7205,7 +7207,7 @@
       </c>
       <c r="H15" s="3">
         <f t="shared" si="3"/>
-        <v>8122.2000000000016</v>
+        <v>7757.0700000000024</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -7224,7 +7226,7 @@
       </c>
       <c r="H16" s="3">
         <f t="shared" si="3"/>
-        <v>8136.4600000000019</v>
+        <v>7771.3300000000027</v>
       </c>
     </row>
     <row r="17" spans="6:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Check cleared for conference
</commit_message>
<xml_diff>
--- a/MIACADA Ledger.xlsx
+++ b/MIACADA Ledger.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="359">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -1237,7 +1237,35 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1610,11 +1638,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="828772688"/>
-        <c:axId val="828774928"/>
+        <c:axId val="697531424"/>
+        <c:axId val="697533104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="828772688"/>
+        <c:axId val="697531424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1657,7 +1685,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="828774928"/>
+        <c:crossAx val="697533104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1665,7 +1693,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="828774928"/>
+        <c:axId val="697533104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1716,7 +1744,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="828772688"/>
+        <c:crossAx val="697531424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2631,7 +2659,7 @@
     <dataField name="Sum of Cost" fld="0" baseField="0" baseItem="0" numFmtId="166"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="16">
+    <format dxfId="20">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -5504,10 +5532,10 @@
   </sheetData>
   <autoFilter ref="E1:E71"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="expression" dxfId="22" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="1" stopIfTrue="1">
       <formula>D1="c"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>NOT(ISBLANK(E1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6810,18 +6838,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E32">
-    <cfRule type="expression" dxfId="20" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="3" stopIfTrue="1">
       <formula>D2="c"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="4">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>NOT(ISBLANK(E2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40:E77">
-    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="1" stopIfTrue="1">
       <formula>D40="c"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="21" priority="2">
       <formula>NOT(ISBLANK(E40))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6835,7 +6863,7 @@
   <dimension ref="A1:M786"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6902,12 +6930,10 @@
       <c r="H2" s="3">
         <v>8381.4599999999991</v>
       </c>
-      <c r="J2" s="3">
-        <v>555.41</v>
-      </c>
+      <c r="J2" s="3"/>
       <c r="K2" s="3">
         <f>SUM(J2:J35)</f>
-        <v>680.41</v>
+        <v>125</v>
       </c>
       <c r="M2" s="3"/>
     </row>
@@ -7295,8 +7321,14 @@
       <c r="A20" s="28">
         <v>43150</v>
       </c>
+      <c r="B20">
+        <v>1349</v>
+      </c>
       <c r="C20" s="20" t="s">
         <v>358</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E20">
         <v>555.41</v>
@@ -7307,27 +7339,45 @@
       </c>
       <c r="H20" s="3">
         <f t="shared" si="3"/>
-        <v>7814.8500000000031</v>
+        <v>7259.4400000000032</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G21" s="3" t="str">
+      <c r="A21" s="28">
+        <v>43152</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="F21">
+        <v>14.26</v>
+      </c>
+      <c r="G21" s="3">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="H21" s="3" t="str">
+        <v>7148.7000000000035</v>
+      </c>
+      <c r="H21" s="3">
         <f t="shared" si="3"/>
-        <v/>
+        <v>7273.7000000000035</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G22" s="3" t="str">
+      <c r="A22" s="28">
+        <v>43154</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="F22">
+        <v>14.26</v>
+      </c>
+      <c r="G22" s="3">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="H22" s="3" t="str">
+        <v>7162.9600000000037</v>
+      </c>
+      <c r="H22" s="3">
         <f t="shared" si="3"/>
-        <v/>
+        <v>7287.9600000000037</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -14972,68 +15022,76 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
+  <conditionalFormatting sqref="E1:E20 E23:E1048576">
+    <cfRule type="expression" dxfId="19" priority="17" stopIfTrue="1">
       <formula>D1="c"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="16">
+    <cfRule type="expression" dxfId="18" priority="18">
       <formula>NOT(ISBLANK(E1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M4">
-    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="15" stopIfTrue="1">
       <formula>L2="c"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="16" priority="16">
       <formula>NOT(ISBLANK(M2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5">
-    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="13" stopIfTrue="1">
       <formula>L5="c"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="14" priority="14">
       <formula>NOT(ISBLANK(M5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="11" stopIfTrue="1">
       <formula>E14="c"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>NOT(ISBLANK(F14))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J4">
-    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
       <formula>I2="c"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>NOT(ISBLANK(J2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="7" stopIfTrue="1">
       <formula>I5="c"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>NOT(ISBLANK(J5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
       <formula>I6="c"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>NOT(ISBLANK(J6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>I7="c"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>NOT(ISBLANK(J7))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21:E22">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+      <formula>D21="c"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>NOT(ISBLANK(E21))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1/22 2nd Push Changes
</commit_message>
<xml_diff>
--- a/MIACADA Ledger.xlsx
+++ b/MIACADA Ledger.xlsx
@@ -1418,63 +1418,7 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="65">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="63">
     <dxf>
       <fill>
         <patternFill>
@@ -1870,6 +1814,48 @@
     <dxf>
       <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2085,11 +2071,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="296934144"/>
-        <c:axId val="301018416"/>
+        <c:axId val="301778896"/>
+        <c:axId val="301780576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="296934144"/>
+        <c:axId val="301778896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2132,7 +2118,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301018416"/>
+        <c:crossAx val="301780576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2140,7 +2126,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="301018416"/>
+        <c:axId val="301780576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2191,7 +2177,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296934144"/>
+        <c:crossAx val="301778896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2454,11 +2440,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="301021776"/>
-        <c:axId val="301022336"/>
+        <c:axId val="405809536"/>
+        <c:axId val="303049616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="301021776"/>
+        <c:axId val="405809536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2501,7 +2487,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301022336"/>
+        <c:crossAx val="303049616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2509,7 +2495,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="301022336"/>
+        <c:axId val="303049616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2560,7 +2546,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301021776"/>
+        <c:crossAx val="405809536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3500,11 +3486,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="399710000"/>
-        <c:axId val="399710560"/>
+        <c:axId val="417223440"/>
+        <c:axId val="417224000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="399710000"/>
+        <c:axId val="417223440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3547,7 +3533,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399710560"/>
+        <c:crossAx val="417224000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3555,7 +3541,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="399710560"/>
+        <c:axId val="417224000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3606,7 +3592,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399710000"/>
+        <c:crossAx val="417223440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6819,7 +6805,7 @@
     <dataField name="Sum of Cost" fld="0" baseField="0" baseItem="0" numFmtId="166"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="64">
+    <format dxfId="56">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -9974,10 +9960,10 @@
   </sheetData>
   <autoFilter ref="E1:E71"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="expression" dxfId="61" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="1" stopIfTrue="1">
       <formula>D1="c"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="2">
+    <cfRule type="expression" dxfId="61" priority="2">
       <formula>NOT(ISBLANK(E1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11289,18 +11275,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E32">
-    <cfRule type="expression" dxfId="59" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="3" stopIfTrue="1">
       <formula>D2="c"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="4">
+    <cfRule type="expression" dxfId="59" priority="4">
       <formula>NOT(ISBLANK(E2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40:E77">
-    <cfRule type="expression" dxfId="57" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="1" stopIfTrue="1">
       <formula>D40="c"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="2">
+    <cfRule type="expression" dxfId="57" priority="2">
       <formula>NOT(ISBLANK(E40))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11413,7 +11399,7 @@
         <v>8321.41</v>
       </c>
       <c r="H3" s="3">
-        <f>IF(D3="C",H2-E3+F3,H2+F3)</f>
+        <f t="shared" ref="H3:H10" si="0">IF(D3="C",H2-E3+F3,H2+F3)</f>
         <v>8321.41</v>
       </c>
       <c r="J3" s="3">
@@ -11437,7 +11423,7 @@
         <v>8335.67</v>
       </c>
       <c r="H4" s="3">
-        <f>IF(D4="C",H3-E4+F4,H3+F4)</f>
+        <f t="shared" si="0"/>
         <v>8335.67</v>
       </c>
       <c r="J4" s="3"/>
@@ -11459,7 +11445,7 @@
         <v>8364.19</v>
       </c>
       <c r="H5" s="3">
-        <f>IF(D5="C",H4-E5+F5,H4+F5)</f>
+        <f t="shared" si="0"/>
         <v>8364.19</v>
       </c>
       <c r="J5" s="3"/>
@@ -11481,7 +11467,7 @@
         <v>8406.9700000000012</v>
       </c>
       <c r="H6" s="3">
-        <f>IF(D6="C",H5-E6+F6,H5+F6)</f>
+        <f t="shared" si="0"/>
         <v>8406.9700000000012</v>
       </c>
       <c r="J6" s="24"/>
@@ -11503,7 +11489,7 @@
         <v>8449.7500000000018</v>
       </c>
       <c r="H7" s="3">
-        <f>IF(D7="C",H6-E7+F7,H6+F7)</f>
+        <f t="shared" si="0"/>
         <v>8449.7500000000018</v>
       </c>
       <c r="J7" s="3"/>
@@ -11524,7 +11510,7 @@
         <v>8478.2700000000023</v>
       </c>
       <c r="H8" s="3">
-        <f>IF(D8="C",H7-E8+F8,H7+F8)</f>
+        <f t="shared" si="0"/>
         <v>8478.2700000000023</v>
       </c>
       <c r="M8" s="3"/>
@@ -11545,7 +11531,7 @@
         <v>8492.5300000000025</v>
       </c>
       <c r="H9" s="3">
-        <f>IF(D9="C",H8-E9+F9,H8+F9)</f>
+        <f t="shared" si="0"/>
         <v>8492.5300000000025</v>
       </c>
     </row>
@@ -11571,7 +11557,7 @@
         <v>8098.4700000000021</v>
       </c>
       <c r="H10" s="3">
-        <f>IF(D10="C",H9-E10+F10,H9+F10)</f>
+        <f t="shared" si="0"/>
         <v>8098.4700000000021</v>
       </c>
       <c r="M10" s="3"/>
@@ -11591,7 +11577,7 @@
         <v>8112.7300000000023</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" ref="H11:H69" si="0">IF(D11="C",H10-E11+F11,H10+F11)</f>
+        <f t="shared" ref="H11:H69" si="1">IF(D11="C",H10-E11+F11,H10+F11)</f>
         <v>8112.7300000000023</v>
       </c>
       <c r="J11" s="3"/>
@@ -11612,7 +11598,7 @@
         <v>8141.2500000000027</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8141.2500000000027</v>
       </c>
     </row>
@@ -11637,7 +11623,7 @@
         <v>8047.8900000000031</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8047.8900000000031</v>
       </c>
       <c r="J13" s="23"/>
@@ -11665,7 +11651,7 @@
         <v>7807.7600000000029</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7807.7600000000029</v>
       </c>
       <c r="L14" s="3"/>
@@ -11685,7 +11671,7 @@
         <v>7822.0200000000032</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7822.0200000000032</v>
       </c>
     </row>
@@ -11704,7 +11690,7 @@
         <v>7836.2800000000034</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7836.2800000000034</v>
       </c>
     </row>
@@ -11723,7 +11709,7 @@
         <v>7851.2800000000034</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7851.2800000000034</v>
       </c>
     </row>
@@ -11742,7 +11728,7 @@
         <v>7865.5400000000036</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7865.5400000000036</v>
       </c>
     </row>
@@ -11761,7 +11747,7 @@
         <v>7879.8000000000038</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7879.8000000000038</v>
       </c>
     </row>
@@ -11786,7 +11772,7 @@
         <v>7324.390000000004</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7324.390000000004</v>
       </c>
     </row>
@@ -11805,7 +11791,7 @@
         <v>7338.6500000000042</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7338.6500000000042</v>
       </c>
     </row>
@@ -11824,7 +11810,7 @@
         <v>7352.9100000000044</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7352.9100000000044</v>
       </c>
     </row>
@@ -11843,7 +11829,7 @@
         <v>7415.7200000000048</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7415.7200000000048</v>
       </c>
       <c r="K23" s="3"/>
@@ -11863,7 +11849,7 @@
         <v>7589.5900000000047</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7589.5900000000047</v>
       </c>
     </row>
@@ -11882,7 +11868,7 @@
         <v>7652.4000000000051</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7652.4000000000051</v>
       </c>
     </row>
@@ -11907,7 +11893,7 @@
         <v>7512.4000000000051</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7512.4000000000051</v>
       </c>
     </row>
@@ -11932,7 +11918,7 @@
         <v>7412.4000000000051</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7412.4000000000051</v>
       </c>
     </row>
@@ -11957,7 +11943,7 @@
         <v>7272.4000000000051</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7272.4000000000051</v>
       </c>
     </row>
@@ -11976,7 +11962,7 @@
         <v>7335.2100000000055</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7335.2100000000055</v>
       </c>
     </row>
@@ -11995,7 +11981,7 @@
         <v>7769.1100000000051</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7769.1100000000051</v>
       </c>
     </row>
@@ -12014,7 +12000,7 @@
         <v>7783.3700000000053</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7783.3700000000053</v>
       </c>
     </row>
@@ -12033,7 +12019,7 @@
         <v>7966.0300000000052</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7966.0300000000052</v>
       </c>
     </row>
@@ -12052,7 +12038,7 @@
         <v>8057.3600000000051</v>
       </c>
       <c r="H33" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8057.3600000000051</v>
       </c>
     </row>
@@ -12071,7 +12057,7 @@
         <v>8085.8800000000056</v>
       </c>
       <c r="H34" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8085.8800000000056</v>
       </c>
     </row>
@@ -12093,7 +12079,7 @@
         <v>7945.8800000000056</v>
       </c>
       <c r="H35" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7945.8800000000056</v>
       </c>
     </row>
@@ -12112,7 +12098,7 @@
         <v>8071.2000000000053</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8071.2000000000053</v>
       </c>
     </row>
@@ -12131,7 +12117,7 @@
         <v>8182.2600000000057</v>
       </c>
       <c r="H37" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8182.2600000000057</v>
       </c>
     </row>
@@ -12150,7 +12136,7 @@
         <v>8196.5200000000059</v>
       </c>
       <c r="H38" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8196.5200000000059</v>
       </c>
     </row>
@@ -12175,7 +12161,7 @@
         <v>8131.5200000000059</v>
       </c>
       <c r="H39" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8131.5200000000059</v>
       </c>
     </row>
@@ -12194,7 +12180,7 @@
         <v>8174.3000000000056</v>
       </c>
       <c r="H40" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8174.3000000000056</v>
       </c>
     </row>
@@ -12213,7 +12199,7 @@
         <v>8237.110000000006</v>
       </c>
       <c r="H41" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8237.110000000006</v>
       </c>
     </row>
@@ -12232,7 +12218,7 @@
         <v>8407.110000000006</v>
       </c>
       <c r="H42" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8407.110000000006</v>
       </c>
     </row>
@@ -12251,7 +12237,7 @@
         <v>8469.9200000000055</v>
       </c>
       <c r="H43" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8469.9200000000055</v>
       </c>
     </row>
@@ -12270,7 +12256,7 @@
         <v>8595.5400000000063</v>
       </c>
       <c r="H44" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8595.5400000000063</v>
       </c>
     </row>
@@ -12289,7 +12275,7 @@
         <v>8735.4200000000055</v>
       </c>
       <c r="H45" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8735.4200000000055</v>
       </c>
     </row>
@@ -12308,7 +12294,7 @@
         <v>8846.1800000000057</v>
       </c>
       <c r="H46" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8846.1800000000057</v>
       </c>
     </row>
@@ -12327,7 +12313,7 @@
         <v>8923.2500000000055</v>
       </c>
       <c r="H47" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8923.2500000000055</v>
       </c>
     </row>
@@ -12346,7 +12332,7 @@
         <v>9238.2500000000055</v>
       </c>
       <c r="H48" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9238.2500000000055</v>
       </c>
     </row>
@@ -12365,7 +12351,7 @@
         <v>9252.5100000000057</v>
       </c>
       <c r="H49" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9252.5100000000057</v>
       </c>
     </row>
@@ -12384,7 +12370,7 @@
         <v>9315.3200000000052</v>
       </c>
       <c r="H50" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9315.3200000000052</v>
       </c>
     </row>
@@ -12403,7 +12389,7 @@
         <v>9467.940000000006</v>
       </c>
       <c r="H51" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9467.940000000006</v>
       </c>
     </row>
@@ -12422,7 +12408,7 @@
         <v>9796.2500000000055</v>
       </c>
       <c r="H52" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9796.2500000000055</v>
       </c>
     </row>
@@ -12441,7 +12427,7 @@
         <v>9936.1300000000047</v>
       </c>
       <c r="H53" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9936.1300000000047</v>
       </c>
     </row>
@@ -12460,7 +12446,7 @@
         <v>10313.910000000005</v>
       </c>
       <c r="H54" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10313.910000000005</v>
       </c>
     </row>
@@ -12479,7 +12465,7 @@
         <v>10565.150000000005</v>
       </c>
       <c r="H55" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10565.150000000005</v>
       </c>
     </row>
@@ -12498,7 +12484,7 @@
         <v>10627.960000000005</v>
       </c>
       <c r="H56" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10627.960000000005</v>
       </c>
     </row>
@@ -12517,7 +12503,7 @@
         <v>12592.960000000005</v>
       </c>
       <c r="H57" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12592.960000000005</v>
       </c>
     </row>
@@ -12536,7 +12522,7 @@
         <v>12704.020000000004</v>
       </c>
       <c r="H58" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12704.020000000004</v>
       </c>
     </row>
@@ -12561,7 +12547,7 @@
         <v>12454.020000000004</v>
       </c>
       <c r="H59" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12454.020000000004</v>
       </c>
     </row>
@@ -12580,7 +12566,7 @@
         <v>13271.170000000004</v>
       </c>
       <c r="H60" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13271.170000000004</v>
       </c>
     </row>
@@ -12599,7 +12585,7 @@
         <v>13459.300000000003</v>
       </c>
       <c r="H61" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13459.300000000003</v>
       </c>
     </row>
@@ -12618,7 +12604,7 @@
         <v>14359.600000000002</v>
       </c>
       <c r="H62" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14359.600000000002</v>
       </c>
     </row>
@@ -12643,7 +12629,7 @@
         <v>14109.600000000002</v>
       </c>
       <c r="H63" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14109.600000000002</v>
       </c>
     </row>
@@ -12668,7 +12654,7 @@
         <v>13975.800000000003</v>
       </c>
       <c r="H64" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13975.800000000003</v>
       </c>
     </row>
@@ -12687,7 +12673,7 @@
         <v>14052.870000000003</v>
       </c>
       <c r="H65" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14052.870000000003</v>
       </c>
     </row>
@@ -12706,7 +12692,7 @@
         <v>14366.620000000003</v>
       </c>
       <c r="H66" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14366.620000000003</v>
       </c>
     </row>
@@ -12725,7 +12711,7 @@
         <v>14792.650000000003</v>
       </c>
       <c r="H67" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14792.650000000003</v>
       </c>
     </row>
@@ -12744,7 +12730,7 @@
         <v>14855.160000000003</v>
       </c>
       <c r="H68" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14855.160000000003</v>
       </c>
     </row>
@@ -12769,7 +12755,7 @@
         <v>14778.360000000004</v>
       </c>
       <c r="H69" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14778.360000000004</v>
       </c>
     </row>
@@ -12807,7 +12793,7 @@
         <v>15072.080000000004</v>
       </c>
       <c r="H71" s="3">
-        <f t="shared" ref="H71:H102" si="1">IF(ISBLANK(A71),"",IF(D71="C",H70-E71+F71,H70+F71))</f>
+        <f t="shared" ref="H71:H102" si="2">IF(ISBLANK(A71),"",IF(D71="C",H70-E71+F71,H70+F71))</f>
         <v>15072.080000000004</v>
       </c>
     </row>
@@ -12832,7 +12818,7 @@
         <v>14612.080000000004</v>
       </c>
       <c r="H72" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14612.080000000004</v>
       </c>
     </row>
@@ -12857,7 +12843,7 @@
         <v>14547.080000000004</v>
       </c>
       <c r="H73" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14547.080000000004</v>
       </c>
     </row>
@@ -12882,7 +12868,7 @@
         <v>14407.080000000004</v>
       </c>
       <c r="H74" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14407.080000000004</v>
       </c>
     </row>
@@ -12901,7 +12887,7 @@
         <v>14720.830000000004</v>
       </c>
       <c r="H75" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14720.830000000004</v>
       </c>
     </row>
@@ -12920,7 +12906,7 @@
         <v>14909.260000000004</v>
       </c>
       <c r="H76" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14909.260000000004</v>
       </c>
     </row>
@@ -12939,7 +12925,7 @@
         <v>16232.550000000003</v>
       </c>
       <c r="H77" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16232.550000000003</v>
       </c>
     </row>
@@ -12958,7 +12944,7 @@
         <v>16357.870000000003</v>
       </c>
       <c r="H78" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16357.870000000003</v>
       </c>
     </row>
@@ -12977,7 +12963,7 @@
         <v>16747.870000000003</v>
       </c>
       <c r="H79" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16747.870000000003</v>
       </c>
     </row>
@@ -13002,7 +12988,7 @@
         <v>16697.870000000003</v>
       </c>
       <c r="H80" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16697.870000000003</v>
       </c>
     </row>
@@ -13027,7 +13013,7 @@
         <v>16141.940000000002</v>
       </c>
       <c r="H81" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16141.940000000002</v>
       </c>
     </row>
@@ -13046,7 +13032,7 @@
         <v>16460.86</v>
       </c>
       <c r="H82" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16460.86</v>
       </c>
     </row>
@@ -13065,7 +13051,7 @@
         <v>17480.86</v>
       </c>
       <c r="H83" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17480.86</v>
       </c>
     </row>
@@ -13084,7 +13070,7 @@
         <v>17795.53</v>
       </c>
       <c r="H84" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17795.53</v>
       </c>
     </row>
@@ -13103,7 +13089,7 @@
         <v>18235.82</v>
       </c>
       <c r="H85" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18235.82</v>
       </c>
     </row>
@@ -13122,7 +13108,7 @@
         <v>18389.66</v>
       </c>
       <c r="H86" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18389.66</v>
       </c>
     </row>
@@ -13147,7 +13133,7 @@
         <v>13139.66</v>
       </c>
       <c r="H87" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13139.66</v>
       </c>
     </row>
@@ -13172,7 +13158,7 @@
         <v>12539.66</v>
       </c>
       <c r="H88" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12539.66</v>
       </c>
     </row>
@@ -13197,7 +13183,7 @@
         <v>11782.85</v>
       </c>
       <c r="H89" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11782.85</v>
       </c>
     </row>
@@ -13222,7 +13208,7 @@
         <v>11582.85</v>
       </c>
       <c r="H90" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11582.85</v>
       </c>
     </row>
@@ -13247,7 +13233,7 @@
         <v>11532.85</v>
       </c>
       <c r="H91" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11532.85</v>
       </c>
     </row>
@@ -13266,7 +13252,7 @@
         <v>11575.630000000001</v>
       </c>
       <c r="H92" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11575.630000000001</v>
       </c>
     </row>
@@ -13285,7 +13271,7 @@
         <v>11589.890000000001</v>
       </c>
       <c r="H93" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11589.890000000001</v>
       </c>
     </row>
@@ -13304,7 +13290,7 @@
         <v>12109.890000000001</v>
       </c>
       <c r="H94" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12109.890000000001</v>
       </c>
     </row>
@@ -13329,7 +13315,7 @@
         <v>11609.890000000001</v>
       </c>
       <c r="H95" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11609.890000000001</v>
       </c>
     </row>
@@ -13348,7 +13334,7 @@
         <v>11624.150000000001</v>
       </c>
       <c r="H96" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11624.150000000001</v>
       </c>
     </row>
@@ -13367,7 +13353,7 @@
         <v>11638.410000000002</v>
       </c>
       <c r="H97" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11638.410000000002</v>
       </c>
     </row>
@@ -13386,7 +13372,7 @@
         <v>11652.670000000002</v>
       </c>
       <c r="H98" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11652.670000000002</v>
       </c>
     </row>
@@ -13405,7 +13391,7 @@
         <v>11666.930000000002</v>
       </c>
       <c r="H99" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11666.930000000002</v>
       </c>
     </row>
@@ -13424,7 +13410,7 @@
         <v>11681.190000000002</v>
       </c>
       <c r="H100" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11681.190000000002</v>
       </c>
     </row>
@@ -13443,7 +13429,7 @@
         <v>11695.450000000003</v>
       </c>
       <c r="H101" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11695.450000000003</v>
       </c>
     </row>
@@ -13462,7 +13448,7 @@
         <v>11709.710000000003</v>
       </c>
       <c r="H102" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11709.710000000003</v>
       </c>
     </row>
@@ -13487,7 +13473,7 @@
         <v>11609.710000000003</v>
       </c>
       <c r="H103" s="3">
-        <f t="shared" ref="H103" si="2">IF(ISBLANK(A103),"",IF(D103="C",H102-E103+F103,H102+F103))</f>
+        <f t="shared" ref="H103" si="3">IF(ISBLANK(A103),"",IF(D103="C",H102-E103+F103,H102+F103))</f>
         <v>11609.710000000003</v>
       </c>
     </row>
@@ -13506,7 +13492,7 @@
         <v>11623.970000000003</v>
       </c>
       <c r="H104" s="3">
-        <f>IF(ISBLANK(A104),"",IF(D104="C",H103-E104+F104,H103+F104))</f>
+        <f t="shared" ref="H104:H135" si="4">IF(ISBLANK(A104),"",IF(D104="C",H103-E104+F104,H103+F104))</f>
         <v>11623.970000000003</v>
       </c>
     </row>
@@ -13525,7 +13511,7 @@
         <v>11638.230000000003</v>
       </c>
       <c r="H105" s="3">
-        <f>IF(ISBLANK(A105),"",IF(D105="C",H104-E105+F105,H104+F105))</f>
+        <f t="shared" si="4"/>
         <v>11638.230000000003</v>
       </c>
     </row>
@@ -13544,7 +13530,7 @@
         <v>11923.230000000003</v>
       </c>
       <c r="H106" s="3">
-        <f>IF(ISBLANK(A106),"",IF(D106="C",H105-E106+F106,H105+F106))</f>
+        <f t="shared" si="4"/>
         <v>11923.230000000003</v>
       </c>
     </row>
@@ -13563,7 +13549,7 @@
         <v>11937.490000000003</v>
       </c>
       <c r="H107" s="3">
-        <f>IF(ISBLANK(A107),"",IF(D107="C",H106-E107+F107,H106+F107))</f>
+        <f t="shared" si="4"/>
         <v>11937.490000000003</v>
       </c>
     </row>
@@ -13582,7 +13568,7 @@
         <v>11951.750000000004</v>
       </c>
       <c r="H108" s="3">
-        <f>IF(ISBLANK(A108),"",IF(D108="C",H107-E108+F108,H107+F108))</f>
+        <f t="shared" si="4"/>
         <v>11951.750000000004</v>
       </c>
     </row>
@@ -13601,7 +13587,7 @@
         <v>12041.750000000004</v>
       </c>
       <c r="H109" s="3">
-        <f>IF(ISBLANK(A109),"",IF(D109="C",H108-E109+F109,H108+F109))</f>
+        <f t="shared" si="4"/>
         <v>12041.750000000004</v>
       </c>
     </row>
@@ -13626,7 +13612,7 @@
         <v>10041.750000000004</v>
       </c>
       <c r="H110" s="3">
-        <f>IF(ISBLANK(A110),"",IF(D110="C",H109-E110+F110,H109+F110))</f>
+        <f t="shared" si="4"/>
         <v>10041.750000000004</v>
       </c>
     </row>
@@ -13645,7 +13631,7 @@
         <v>10070.270000000004</v>
       </c>
       <c r="H111" s="3">
-        <f>IF(ISBLANK(A111),"",IF(D111="C",H110-E111+F111,H110+F111))</f>
+        <f t="shared" si="4"/>
         <v>10070.270000000004</v>
       </c>
     </row>
@@ -13670,7 +13656,7 @@
         <v>9670.2700000000041</v>
       </c>
       <c r="H112" s="3">
-        <f>IF(ISBLANK(A112),"",IF(D112="C",H111-E112+F112,H111+F112))</f>
+        <f t="shared" si="4"/>
         <v>9670.2700000000041</v>
       </c>
     </row>
@@ -13689,7 +13675,7 @@
         <v>9757.0500000000047</v>
       </c>
       <c r="H113" s="3">
-        <f>IF(ISBLANK(A113),"",IF(D113="C",H112-E113+F113,H112+F113))</f>
+        <f t="shared" si="4"/>
         <v>9757.0500000000047</v>
       </c>
     </row>
@@ -13708,7 +13694,7 @@
         <v>9771.3100000000049</v>
       </c>
       <c r="H114" s="3">
-        <f>IF(ISBLANK(A114),"",IF(D114="C",H113-E114+F114,H113+F114))</f>
+        <f t="shared" si="4"/>
         <v>9771.3100000000049</v>
       </c>
     </row>
@@ -13727,7 +13713,7 @@
         <v>9785.5700000000052</v>
       </c>
       <c r="H115" s="3">
-        <f>IF(ISBLANK(A115),"",IF(D115="C",H114-E115+F115,H114+F115))</f>
+        <f t="shared" si="4"/>
         <v>9785.5700000000052</v>
       </c>
     </row>
@@ -13746,7 +13732,7 @@
         <v>9799.8300000000054</v>
       </c>
       <c r="H116" s="3">
-        <f>IF(ISBLANK(A116),"",IF(D116="C",H115-E116+F116,H115+F116))</f>
+        <f t="shared" si="4"/>
         <v>9799.8300000000054</v>
       </c>
     </row>
@@ -13771,7 +13757,7 @@
         <v>9735.8300000000054</v>
       </c>
       <c r="H117" s="3">
-        <f>IF(ISBLANK(A117),"",IF(D117="C",H116-E117+F117,H116+F117))</f>
+        <f t="shared" si="4"/>
         <v>9735.8300000000054</v>
       </c>
     </row>
@@ -13790,7 +13776,7 @@
         <v>9765.8300000000054</v>
       </c>
       <c r="H118" s="3">
-        <f>IF(ISBLANK(A118),"",IF(D118="C",H117-E118+F118,H117+F118))</f>
+        <f t="shared" si="4"/>
         <v>9765.8300000000054</v>
       </c>
     </row>
@@ -13815,7 +13801,7 @@
         <v>9704.8300000000054</v>
       </c>
       <c r="H119" s="3">
-        <f>IF(ISBLANK(A119),"",IF(D119="C",H118-E119+F119,H118+F119))</f>
+        <f t="shared" si="4"/>
         <v>9704.8300000000054</v>
       </c>
     </row>
@@ -13840,7 +13826,7 @@
         <v>9472.3800000000047</v>
       </c>
       <c r="H120" s="3">
-        <f>IF(ISBLANK(A120),"",IF(D120="C",H119-E120+F120,H119+F120))</f>
+        <f t="shared" si="4"/>
         <v>9472.3800000000047</v>
       </c>
     </row>
@@ -13859,7 +13845,7 @@
         <v>9486.6400000000049</v>
       </c>
       <c r="H121" s="3">
-        <f>IF(ISBLANK(A121),"",IF(D121="C",H120-E121+F121,H120+F121))</f>
+        <f t="shared" si="4"/>
         <v>9486.6400000000049</v>
       </c>
     </row>
@@ -13884,7 +13870,7 @@
         <v>9206.5400000000045</v>
       </c>
       <c r="H122" s="3">
-        <f>IF(ISBLANK(A122),"",IF(D122="C",H121-E122+F122,H121+F122))</f>
+        <f t="shared" si="4"/>
         <v>9206.5400000000045</v>
       </c>
     </row>
@@ -13909,7 +13895,7 @@
         <v>8706.5400000000045</v>
       </c>
       <c r="H123" s="3">
-        <f>IF(ISBLANK(A123),"",IF(D123="C",H122-E123+F123,H122+F123))</f>
+        <f t="shared" si="4"/>
         <v>8706.5400000000045</v>
       </c>
     </row>
@@ -13928,7 +13914,7 @@
         <v>8721.5400000000045</v>
       </c>
       <c r="H124" s="3">
-        <f>IF(ISBLANK(A124),"",IF(D124="C",H123-E124+F124,H123+F124))</f>
+        <f t="shared" si="4"/>
         <v>8721.5400000000045</v>
       </c>
     </row>
@@ -13947,7 +13933,7 @@
         <v>8750.0600000000049</v>
       </c>
       <c r="H125" s="3">
-        <f>IF(ISBLANK(A125),"",IF(D125="C",H124-E125+F125,H124+F125))</f>
+        <f t="shared" si="4"/>
         <v>8750.0600000000049</v>
       </c>
     </row>
@@ -13972,7 +13958,7 @@
         <v>8665.0600000000049</v>
       </c>
       <c r="H126" s="3">
-        <f>IF(ISBLANK(A126),"",IF(D126="C",H125-E126+F126,H125+F126))</f>
+        <f t="shared" si="4"/>
         <v>8665.0600000000049</v>
       </c>
     </row>
@@ -13991,7 +13977,7 @@
         <v>8679.3200000000052</v>
       </c>
       <c r="H127" s="3">
-        <f>IF(ISBLANK(A127),"",IF(D127="C",H126-E127+F127,H126+F127))</f>
+        <f t="shared" si="4"/>
         <v>8679.3200000000052</v>
       </c>
     </row>
@@ -14016,7 +14002,7 @@
         <v>8620.3200000000052</v>
       </c>
       <c r="H128" s="3">
-        <f>IF(ISBLANK(A128),"",IF(D128="C",H127-E128+F128,H127+F128))</f>
+        <f t="shared" si="4"/>
         <v>8620.3200000000052</v>
       </c>
     </row>
@@ -14042,7 +14028,7 @@
         <v>7805.9200000000055</v>
       </c>
       <c r="H129" s="3">
-        <f>IF(ISBLANK(A129),"",IF(D129="C",H128-E129+F129,H128+F129))</f>
+        <f t="shared" si="4"/>
         <v>7805.9200000000055</v>
       </c>
     </row>
@@ -14068,7 +14054,7 @@
         <v>7751.2500000000055</v>
       </c>
       <c r="H130" s="3">
-        <f>IF(ISBLANK(A130),"",IF(D130="C",H129-E130+F130,H129+F130))</f>
+        <f t="shared" si="4"/>
         <v>7751.2500000000055</v>
       </c>
     </row>
@@ -14087,7 +14073,7 @@
         <v>7765.5100000000057</v>
       </c>
       <c r="H131" s="3">
-        <f>IF(ISBLANK(A131),"",IF(D131="C",H130-E131+F131,H130+F131))</f>
+        <f t="shared" si="4"/>
         <v>7765.5100000000057</v>
       </c>
     </row>
@@ -14106,7 +14092,7 @@
         <v>7779.7700000000059</v>
       </c>
       <c r="H132" s="3">
-        <f>IF(ISBLANK(A132),"",IF(D132="C",H131-E132+F132,H131+F132))</f>
+        <f t="shared" si="4"/>
         <v>7779.7700000000059</v>
       </c>
     </row>
@@ -14131,7 +14117,7 @@
         <v>7029.7700000000059</v>
       </c>
       <c r="H133" s="3">
-        <f>IF(ISBLANK(A133),"",IF(D133="C",H132-E133+F133,H132+F133))</f>
+        <f t="shared" si="4"/>
         <v>7029.7700000000059</v>
       </c>
     </row>
@@ -14156,7 +14142,7 @@
         <v>6779.7700000000059</v>
       </c>
       <c r="H134" s="3">
-        <f>IF(ISBLANK(A134),"",IF(D134="C",H133-E134+F134,H133+F134))</f>
+        <f t="shared" si="4"/>
         <v>6779.7700000000059</v>
       </c>
     </row>
@@ -14181,7 +14167,7 @@
         <v>6129.7700000000059</v>
       </c>
       <c r="H135" s="3">
-        <f>IF(ISBLANK(A135),"",IF(D135="C",H134-E135+F135,H134+F135))</f>
+        <f t="shared" si="4"/>
         <v>6129.7700000000059</v>
       </c>
     </row>
@@ -14200,7 +14186,7 @@
         <v>6144.0300000000061</v>
       </c>
       <c r="H136" s="3">
-        <f>IF(ISBLANK(A136),"",IF(D136="C",H135-E136+F136,H135+F136))</f>
+        <f t="shared" ref="H136:H167" si="5">IF(ISBLANK(A136),"",IF(D136="C",H135-E136+F136,H135+F136))</f>
         <v>6144.0300000000061</v>
       </c>
     </row>
@@ -14219,7 +14205,7 @@
         <v>6158.2900000000063</v>
       </c>
       <c r="H137" s="3">
-        <f>IF(ISBLANK(A137),"",IF(D137="C",H136-E137+F137,H136+F137))</f>
+        <f t="shared" si="5"/>
         <v>6158.2900000000063</v>
       </c>
     </row>
@@ -14244,7 +14230,7 @@
         <v>6033.2900000000063</v>
       </c>
       <c r="H138" s="3">
-        <f>IF(ISBLANK(A138),"",IF(D138="C",H137-E138+F138,H137+F138))</f>
+        <f t="shared" si="5"/>
         <v>6033.2900000000063</v>
       </c>
     </row>
@@ -14263,7 +14249,7 @@
         <v>6061.8100000000068</v>
       </c>
       <c r="H139" s="3">
-        <f>IF(ISBLANK(A139),"",IF(D139="C",H138-E139+F139,H138+F139))</f>
+        <f t="shared" si="5"/>
         <v>6061.8100000000068</v>
       </c>
     </row>
@@ -14282,7 +14268,7 @@
         <v>6090.6400000000067</v>
       </c>
       <c r="H140" s="3">
-        <f>IF(ISBLANK(A140),"",IF(D140="C",H139-E140+F140,H139+F140))</f>
+        <f t="shared" si="5"/>
         <v>6090.6400000000067</v>
       </c>
     </row>
@@ -14307,7 +14293,7 @@
         <v>5965.6400000000067</v>
       </c>
       <c r="H141" s="3">
-        <f>IF(ISBLANK(A141),"",IF(D141="C",H140-E141+F141,H140+F141))</f>
+        <f t="shared" si="5"/>
         <v>5965.6400000000067</v>
       </c>
     </row>
@@ -14332,7 +14318,7 @@
         <v>5465.6400000000067</v>
       </c>
       <c r="H142" s="3">
-        <f>IF(ISBLANK(A142),"",IF(D142="C",H141-E142+F142,H141+F142))</f>
+        <f t="shared" si="5"/>
         <v>5465.6400000000067</v>
       </c>
     </row>
@@ -14351,7 +14337,7 @@
         <v>5479.9000000000069</v>
       </c>
       <c r="H143" s="3">
-        <f>IF(ISBLANK(A143),"",IF(D143="C",H142-E143+F143,H142+F143))</f>
+        <f t="shared" si="5"/>
         <v>5479.9000000000069</v>
       </c>
     </row>
@@ -14370,7 +14356,7 @@
         <v>5494.1600000000071</v>
       </c>
       <c r="H144" s="3">
-        <f>IF(ISBLANK(A144),"",IF(D144="C",H143-E144+F144,H143+F144))</f>
+        <f t="shared" si="5"/>
         <v>5494.1600000000071</v>
       </c>
     </row>
@@ -14395,7 +14381,7 @@
         <v>5208.5600000000068</v>
       </c>
       <c r="H145" s="3">
-        <f>IF(ISBLANK(A145),"",IF(D145="C",H144-E145+F145,H144+F145))</f>
+        <f t="shared" si="5"/>
         <v>5208.5600000000068</v>
       </c>
     </row>
@@ -14414,7 +14400,7 @@
         <v>5222.820000000007</v>
       </c>
       <c r="H146" s="3">
-        <f>IF(ISBLANK(A146),"",IF(D146="C",H145-E146+F146,H145+F146))</f>
+        <f t="shared" si="5"/>
         <v>5222.820000000007</v>
       </c>
     </row>
@@ -14433,7 +14419,7 @@
         <v>5237.0800000000072</v>
       </c>
       <c r="H147" s="3">
-        <f>IF(ISBLANK(A147),"",IF(D147="C",H146-E147+F147,H146+F147))</f>
+        <f t="shared" si="5"/>
         <v>5237.0800000000072</v>
       </c>
     </row>
@@ -14452,7 +14438,7 @@
         <v>5324.1700000000073</v>
       </c>
       <c r="H148" s="3">
-        <f>IF(ISBLANK(A148),"",IF(D148="C",H147-E148+F148,H147+F148))</f>
+        <f t="shared" si="5"/>
         <v>5324.1700000000073</v>
       </c>
     </row>
@@ -14471,7 +14457,7 @@
         <v>5338.4300000000076</v>
       </c>
       <c r="H149" s="3">
-        <f>IF(ISBLANK(A149),"",IF(D149="C",H148-E149+F149,H148+F149))</f>
+        <f t="shared" si="5"/>
         <v>5338.4300000000076</v>
       </c>
     </row>
@@ -14493,7 +14479,7 @@
         <v>5193.4300000000076</v>
       </c>
       <c r="H150" s="3">
-        <f>IF(ISBLANK(A150),"",IF(D150="C",H149-E150+F150,H149+F150))</f>
+        <f t="shared" si="5"/>
         <v>5338.4300000000076</v>
       </c>
     </row>
@@ -14515,7 +14501,7 @@
         <v>5048.4300000000076</v>
       </c>
       <c r="H151" s="3">
-        <f>IF(ISBLANK(A151),"",IF(D151="C",H150-E151+F151,H150+F151))</f>
+        <f t="shared" si="5"/>
         <v>5338.4300000000076</v>
       </c>
     </row>
@@ -14528,7 +14514,7 @@
         <v/>
       </c>
       <c r="H152" s="3" t="str">
-        <f>IF(ISBLANK(A152),"",IF(D152="C",H151-E152+F152,H151+F152))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14541,7 +14527,7 @@
         <v/>
       </c>
       <c r="H153" s="3" t="str">
-        <f>IF(ISBLANK(A153),"",IF(D153="C",H152-E153+F153,H152+F153))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14553,7 +14539,7 @@
         <v/>
       </c>
       <c r="H154" s="3" t="str">
-        <f>IF(ISBLANK(A154),"",IF(D154="C",H153-E154+F154,H153+F154))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14565,7 +14551,7 @@
         <v/>
       </c>
       <c r="H155" s="3" t="str">
-        <f>IF(ISBLANK(A155),"",IF(D155="C",H154-E155+F155,H154+F155))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14575,7 +14561,7 @@
         <v/>
       </c>
       <c r="H156" s="3" t="str">
-        <f>IF(ISBLANK(A156),"",IF(D156="C",H155-E156+F156,H155+F156))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14585,7 +14571,7 @@
         <v/>
       </c>
       <c r="H157" s="3" t="str">
-        <f>IF(ISBLANK(A157),"",IF(D157="C",H156-E157+F157,H156+F157))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14595,7 +14581,7 @@
         <v/>
       </c>
       <c r="H158" s="3" t="str">
-        <f>IF(ISBLANK(A158),"",IF(D158="C",H157-E158+F158,H157+F158))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14605,7 +14591,7 @@
         <v/>
       </c>
       <c r="H159" s="3" t="str">
-        <f>IF(ISBLANK(A159),"",IF(D159="C",H158-E159+F159,H158+F159))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14615,7 +14601,7 @@
         <v/>
       </c>
       <c r="H160" s="3" t="str">
-        <f>IF(ISBLANK(A160),"",IF(D160="C",H159-E160+F160,H159+F160))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14625,7 +14611,7 @@
         <v/>
       </c>
       <c r="H161" s="3" t="str">
-        <f>IF(ISBLANK(A161),"",IF(D161="C",H160-E161+F161,H160+F161))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14635,7 +14621,7 @@
         <v/>
       </c>
       <c r="H162" s="3" t="str">
-        <f>IF(ISBLANK(A162),"",IF(D162="C",H161-E162+F162,H161+F162))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14645,7 +14631,7 @@
         <v/>
       </c>
       <c r="H163" s="3" t="str">
-        <f>IF(ISBLANK(A163),"",IF(D163="C",H162-E163+F163,H162+F163))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14655,7 +14641,7 @@
         <v/>
       </c>
       <c r="H164" s="3" t="str">
-        <f>IF(ISBLANK(A164),"",IF(D164="C",H163-E164+F164,H163+F164))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14665,7 +14651,7 @@
         <v/>
       </c>
       <c r="H165" s="3" t="str">
-        <f>IF(ISBLANK(A165),"",IF(D165="C",H164-E165+F165,H164+F165))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14675,7 +14661,7 @@
         <v/>
       </c>
       <c r="H166" s="3" t="str">
-        <f>IF(ISBLANK(A166),"",IF(D166="C",H165-E166+F166,H165+F166))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14685,7 +14671,7 @@
         <v/>
       </c>
       <c r="H167" s="3" t="str">
-        <f>IF(ISBLANK(A167),"",IF(D167="C",H166-E167+F167,H166+F167))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -14695,7 +14681,7 @@
         <v/>
       </c>
       <c r="H168" s="3" t="str">
-        <f t="shared" ref="H168:H231" si="3">IF(ISBLANK(A168),"",IF(D168="C",H167-E168+F168,H167+F168))</f>
+        <f t="shared" ref="H168:H231" si="6">IF(ISBLANK(A168),"",IF(D168="C",H167-E168+F168,H167+F168))</f>
         <v/>
       </c>
     </row>
@@ -14705,7 +14691,7 @@
         <v/>
       </c>
       <c r="H169" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14715,7 +14701,7 @@
         <v/>
       </c>
       <c r="H170" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14725,7 +14711,7 @@
         <v/>
       </c>
       <c r="H171" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14735,7 +14721,7 @@
         <v/>
       </c>
       <c r="H172" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14745,7 +14731,7 @@
         <v/>
       </c>
       <c r="H173" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14755,7 +14741,7 @@
         <v/>
       </c>
       <c r="H174" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14765,7 +14751,7 @@
         <v/>
       </c>
       <c r="H175" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14775,7 +14761,7 @@
         <v/>
       </c>
       <c r="H176" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14785,7 +14771,7 @@
         <v/>
       </c>
       <c r="H177" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14795,7 +14781,7 @@
         <v/>
       </c>
       <c r="H178" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14805,7 +14791,7 @@
         <v/>
       </c>
       <c r="H179" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14815,7 +14801,7 @@
         <v/>
       </c>
       <c r="H180" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14825,7 +14811,7 @@
         <v/>
       </c>
       <c r="H181" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14835,7 +14821,7 @@
         <v/>
       </c>
       <c r="H182" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14845,7 +14831,7 @@
         <v/>
       </c>
       <c r="H183" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14855,7 +14841,7 @@
         <v/>
       </c>
       <c r="H184" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14865,7 +14851,7 @@
         <v/>
       </c>
       <c r="H185" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14875,7 +14861,7 @@
         <v/>
       </c>
       <c r="H186" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14885,7 +14871,7 @@
         <v/>
       </c>
       <c r="H187" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14895,7 +14881,7 @@
         <v/>
       </c>
       <c r="H188" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14905,7 +14891,7 @@
         <v/>
       </c>
       <c r="H189" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14915,7 +14901,7 @@
         <v/>
       </c>
       <c r="H190" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14925,7 +14911,7 @@
         <v/>
       </c>
       <c r="H191" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14935,7 +14921,7 @@
         <v/>
       </c>
       <c r="H192" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14945,7 +14931,7 @@
         <v/>
       </c>
       <c r="H193" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14955,7 +14941,7 @@
         <v/>
       </c>
       <c r="H194" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14965,7 +14951,7 @@
         <v/>
       </c>
       <c r="H195" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14975,7 +14961,7 @@
         <v/>
       </c>
       <c r="H196" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14985,7 +14971,7 @@
         <v/>
       </c>
       <c r="H197" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -14995,7 +14981,7 @@
         <v/>
       </c>
       <c r="H198" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15005,7 +14991,7 @@
         <v/>
       </c>
       <c r="H199" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15015,7 +15001,7 @@
         <v/>
       </c>
       <c r="H200" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15025,7 +15011,7 @@
         <v/>
       </c>
       <c r="H201" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15035,7 +15021,7 @@
         <v/>
       </c>
       <c r="H202" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15045,7 +15031,7 @@
         <v/>
       </c>
       <c r="H203" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15055,7 +15041,7 @@
         <v/>
       </c>
       <c r="H204" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15065,7 +15051,7 @@
         <v/>
       </c>
       <c r="H205" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15075,7 +15061,7 @@
         <v/>
       </c>
       <c r="H206" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15085,7 +15071,7 @@
         <v/>
       </c>
       <c r="H207" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15095,7 +15081,7 @@
         <v/>
       </c>
       <c r="H208" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15105,7 +15091,7 @@
         <v/>
       </c>
       <c r="H209" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15115,7 +15101,7 @@
         <v/>
       </c>
       <c r="H210" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15125,7 +15111,7 @@
         <v/>
       </c>
       <c r="H211" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15135,7 +15121,7 @@
         <v/>
       </c>
       <c r="H212" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15145,7 +15131,7 @@
         <v/>
       </c>
       <c r="H213" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15155,7 +15141,7 @@
         <v/>
       </c>
       <c r="H214" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15165,7 +15151,7 @@
         <v/>
       </c>
       <c r="H215" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15175,7 +15161,7 @@
         <v/>
       </c>
       <c r="H216" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15185,7 +15171,7 @@
         <v/>
       </c>
       <c r="H217" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15195,7 +15181,7 @@
         <v/>
       </c>
       <c r="H218" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15205,7 +15191,7 @@
         <v/>
       </c>
       <c r="H219" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15215,7 +15201,7 @@
         <v/>
       </c>
       <c r="H220" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15225,7 +15211,7 @@
         <v/>
       </c>
       <c r="H221" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15235,7 +15221,7 @@
         <v/>
       </c>
       <c r="H222" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15245,7 +15231,7 @@
         <v/>
       </c>
       <c r="H223" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15255,7 +15241,7 @@
         <v/>
       </c>
       <c r="H224" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15265,7 +15251,7 @@
         <v/>
       </c>
       <c r="H225" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15275,7 +15261,7 @@
         <v/>
       </c>
       <c r="H226" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15285,7 +15271,7 @@
         <v/>
       </c>
       <c r="H227" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15295,7 +15281,7 @@
         <v/>
       </c>
       <c r="H228" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15305,7 +15291,7 @@
         <v/>
       </c>
       <c r="H229" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15315,7 +15301,7 @@
         <v/>
       </c>
       <c r="H230" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15325,7 +15311,7 @@
         <v/>
       </c>
       <c r="H231" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -15335,7 +15321,7 @@
         <v/>
       </c>
       <c r="H232" s="3" t="str">
-        <f t="shared" ref="H232:H259" si="4">IF(ISBLANK(A232),"",IF(D232="C",H231-E232+F232,H231+F232))</f>
+        <f t="shared" ref="H232:H259" si="7">IF(ISBLANK(A232),"",IF(D232="C",H231-E232+F232,H231+F232))</f>
         <v/>
       </c>
     </row>
@@ -15345,7 +15331,7 @@
         <v/>
       </c>
       <c r="H233" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15355,7 +15341,7 @@
         <v/>
       </c>
       <c r="H234" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15365,7 +15351,7 @@
         <v/>
       </c>
       <c r="H235" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15375,7 +15361,7 @@
         <v/>
       </c>
       <c r="H236" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15385,7 +15371,7 @@
         <v/>
       </c>
       <c r="H237" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15395,7 +15381,7 @@
         <v/>
       </c>
       <c r="H238" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15405,7 +15391,7 @@
         <v/>
       </c>
       <c r="H239" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15415,7 +15401,7 @@
         <v/>
       </c>
       <c r="H240" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15425,7 +15411,7 @@
         <v/>
       </c>
       <c r="H241" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15435,7 +15421,7 @@
         <v/>
       </c>
       <c r="H242" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15445,7 +15431,7 @@
         <v/>
       </c>
       <c r="H243" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15455,7 +15441,7 @@
         <v/>
       </c>
       <c r="H244" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15465,7 +15451,7 @@
         <v/>
       </c>
       <c r="H245" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15475,7 +15461,7 @@
         <v/>
       </c>
       <c r="H246" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15485,7 +15471,7 @@
         <v/>
       </c>
       <c r="H247" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15495,7 +15481,7 @@
         <v/>
       </c>
       <c r="H248" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15505,7 +15491,7 @@
         <v/>
       </c>
       <c r="H249" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15515,7 +15501,7 @@
         <v/>
       </c>
       <c r="H250" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15525,7 +15511,7 @@
         <v/>
       </c>
       <c r="H251" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15535,7 +15521,7 @@
         <v/>
       </c>
       <c r="H252" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15545,7 +15531,7 @@
         <v/>
       </c>
       <c r="H253" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15555,7 +15541,7 @@
         <v/>
       </c>
       <c r="H254" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15565,7 +15551,7 @@
         <v/>
       </c>
       <c r="H255" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15575,7 +15561,7 @@
         <v/>
       </c>
       <c r="H256" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15585,7 +15571,7 @@
         <v/>
       </c>
       <c r="H257" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15595,7 +15581,7 @@
         <v/>
       </c>
       <c r="H258" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15605,7 +15591,7 @@
         <v/>
       </c>
       <c r="H259" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -17836,7 +17822,7 @@
   <dimension ref="A1:M793"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17899,8 +17885,8 @@
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3">
-        <f>'2018'!G151</f>
-        <v>5048.4300000000076</v>
+        <f>'2018'!G151-E2</f>
+        <v>4903.4300000000076</v>
       </c>
       <c r="H2" s="3">
         <f>'2018'!H151-E2</f>
@@ -17934,7 +17920,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3">
         <f>G2-E3+F3</f>
-        <v>4903.4300000000076</v>
+        <v>4758.4300000000076</v>
       </c>
       <c r="H3" s="3">
         <f>IF(D3="C",H2-E3+F3,H2+F3)</f>
@@ -17956,10 +17942,10 @@
       </c>
       <c r="G4" s="3">
         <f>'2019'!G3-E4+F4</f>
-        <v>4917.6900000000078</v>
+        <v>4772.6900000000078</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ref="H4:H67" si="0">IF(D4="C",H3-E4+F4,H3+F4)</f>
+        <f t="shared" ref="H4:H8" si="0">IF(D4="C",H3-E4+F4,H3+F4)</f>
         <v>5062.6900000000078</v>
       </c>
       <c r="J4" s="3"/>
@@ -17978,7 +17964,7 @@
       </c>
       <c r="G5" s="3">
         <f>'2019'!G4-E5+F5</f>
-        <v>4931.950000000008</v>
+        <v>4786.950000000008</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" si="0"/>
@@ -18000,7 +17986,7 @@
       </c>
       <c r="G6" s="3">
         <f>'2019'!G5-E6+F6</f>
-        <v>4946.2100000000082</v>
+        <v>4801.2100000000082</v>
       </c>
       <c r="H6" s="3">
         <f>IF(D6="C",H5-E6+F6,H5+F6)</f>
@@ -18022,7 +18008,7 @@
       </c>
       <c r="G7" s="3">
         <f>'2019'!G6-E7+F7</f>
-        <v>4960.4700000000084</v>
+        <v>4815.4700000000084</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="0"/>
@@ -18047,7 +18033,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3">
         <f>'2019'!G7-E8+F8</f>
-        <v>4815.4700000000084</v>
+        <v>4670.4700000000084</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" si="0"/>

</xml_diff>